<commit_message>
Petite problème de nom de colonne. Problème résolu
</commit_message>
<xml_diff>
--- a/File Name.xlsx
+++ b/File Name.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -454,11 +454,6 @@
           <t>http://dbpedia.org/ontology/birthPlace</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>http://dbpedia.org/property/birthPlace</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -481,11 +476,6 @@
           <t xml:space="preserve">http://dbpedia.org/resource/Kingdom_of_England http://dbpedia.org/resource/Staffordshire http://dbpedia.org/resource/Stourton_Castle </t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t xml:space="preserve">http://dbpedia.org/resource/Kingdom_of_England Stourton Castle, Staffordshire </t>
-        </is>
-      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -504,11 +494,6 @@
         </is>
       </c>
       <c r="D3" t="inlineStr">
-        <is>
-          <t xml:space="preserve">http://dbpedia.org/resource/Andhra_Pradesh </t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
         <is>
           <t xml:space="preserve">http://dbpedia.org/resource/Andhra_Pradesh </t>
         </is>

</xml_diff>

<commit_message>
Export des ontologies, entités de dbpedia de Mtab.
</commit_message>
<xml_diff>
--- a/File Name.xlsx
+++ b/File Name.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -449,11 +449,6 @@
           <t>http://dbpedia.org/ontology/parent</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>http://dbpedia.org/ontology/birthPlace</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -471,11 +466,6 @@
           <t>http://dbpedia.org/resource/Margaret_Pole,_Countess_of_Salisbury</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t xml:space="preserve">http://dbpedia.org/resource/Kingdom_of_England http://dbpedia.org/resource/Staffordshire http://dbpedia.org/resource/Stourton_Castle </t>
-        </is>
-      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -493,9 +483,21 @@
           <t>http://dbpedia.org/resource/Sri</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t xml:space="preserve">http://dbpedia.org/resource/Andhra_Pradesh </t>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>http://dbpedia.org/resource/Y._D._Tiwari</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">http://dbpedia.org/resource/Shillong http://dbpedia.org/resource/Meghalaya </t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>http://dbpedia.org/resource/Father</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Semic Automatic Tool added
</commit_message>
<xml_diff>
--- a/File Name.xlsx
+++ b/File Name.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -449,6 +449,21 @@
           <t>http://dbpedia.org/ontology/parent</t>
         </is>
       </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>http://dbpedia.org/ontology/birthDate</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>http://dbpedia.org/ontology/birthPlace</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>http://dbpedia.org/ontology/deathDate</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -466,6 +481,21 @@
           <t>http://dbpedia.org/resource/Margaret_Pole,_Countess_of_Salisbury</t>
         </is>
       </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">1500-03-12 </t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">http://dbpedia.org/resource/Kingdom_of_England http://dbpedia.org/resource/Staffordshire http://dbpedia.org/resource/Stourton_Castle </t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">1558-11-17 </t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -483,23 +513,13 @@
           <t>http://dbpedia.org/resource/Sri</t>
         </is>
       </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>http://dbpedia.org/resource/Y._D._Tiwari</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t xml:space="preserve">http://dbpedia.org/resource/Shillong http://dbpedia.org/resource/Meghalaya </t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>http://dbpedia.org/resource/Father</t>
-        </is>
-      </c>
+      <c r="D3" t="inlineStr"/>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">http://dbpedia.org/resource/Andhra_Pradesh </t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
First case with same subject column
</commit_message>
<xml_diff>
--- a/File Name.xlsx
+++ b/File Name.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,22 +446,12 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
+          <t>http://dbpedia.org/property/parents</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
           <t>http://dbpedia.org/ontology/parent</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>http://dbpedia.org/ontology/birthDate</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>http://dbpedia.org/ontology/birthPlace</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>http://dbpedia.org/ontology/deathDate</t>
         </is>
       </c>
     </row>
@@ -483,17 +473,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t xml:space="preserve">1500-03-12 </t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t xml:space="preserve">http://dbpedia.org/resource/Kingdom_of_England http://dbpedia.org/resource/Staffordshire http://dbpedia.org/resource/Stourton_Castle </t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t xml:space="preserve">1558-11-17 </t>
+          <t xml:space="preserve">http://dbpedia.org/resource/Margaret_Pole,_Countess_of_Salisbury http://dbpedia.org/resource/Richard_Pole_(courtier) </t>
         </is>
       </c>
     </row>
@@ -513,13 +493,33 @@
           <t>http://dbpedia.org/resource/Sri</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr"/>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t xml:space="preserve">http://dbpedia.org/resource/Andhra_Pradesh </t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr"/>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">http://dbpedia.org/resource/Shri http://dbpedia.org/resource/Shrimati </t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>http://dbpedia.org/resource/Y._D._Tiwari</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">http://dbpedia.org/resource/Meghalaya http://dbpedia.org/resource/Shillong </t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Father: Pandit Hari Govind Tiwari Mother: Rajkunwar </t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>http://dbpedia.org/resource/Father</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Toutes les questions ont été faites avec Mtab.
</commit_message>
<xml_diff>
--- a/File Name.xlsx
+++ b/File Name.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:E42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,90 +436,812 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>http://dbpedia.org/ontology/Person</t>
+          <t>Core Attribute</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>http://dbpedia.org/ontology/birthDate</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>http://dbpedia.org/ontology/deathDate</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>http://dbpedia.org/ontology/birthPlace</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
           <t>http://dbpedia.org/ontology/deathPlace</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>http://dbpedia.org/property/parents</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>http://dbpedia.org/ontology/parent</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>http://dbpedia.org/resource/Reginald_Pole</t>
+          <t>http://dbpedia.org/resource/Nugent_Everard</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>http://dbpedia.org/resource/London</t>
+          <t>http://dbpedia.org/resource/1849</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>http://dbpedia.org/resource/Margaret_Pole,_Countess_of_Salisbury</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t xml:space="preserve">http://dbpedia.org/resource/Margaret_Pole,_Countess_of_Salisbury http://dbpedia.org/resource/Richard_Pole_(courtier) </t>
-        </is>
-      </c>
+          <t>http://dbpedia.org/resource/1929</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>http://dbpedia.org/resource/R._R._Sundara_Rao</t>
+          <t>http://dbpedia.org/resource/No%C3%ABl_Bowater</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>http://dbpedia.org/resource/Tamil_Nadu</t>
+          <t>http://dbpedia.org/resource/12-12-12</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>http://dbpedia.org/resource/Sri</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t xml:space="preserve">http://dbpedia.org/resource/Shri http://dbpedia.org/resource/Shrimati </t>
-        </is>
-      </c>
+          <t>http://dbpedia.org/resource/22_(number)</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr"/>
+      <c r="E3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>http://dbpedia.org/resource/Y._D._Tiwari</t>
+          <t>http://dbpedia.org/resource/Milton_Sharp</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t xml:space="preserve">http://dbpedia.org/resource/Meghalaya http://dbpedia.org/resource/Shillong </t>
+          <t>http://dbpedia.org/resource/1856</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t xml:space="preserve">Father: Pandit Hari Govind Tiwari Mother: Rajkunwar </t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>http://dbpedia.org/resource/Father</t>
-        </is>
-      </c>
+          <t>http://dbpedia.org/resource/1924</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr"/>
+      <c r="E4" t="inlineStr"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>http://dbpedia.org/resource/Merrik_Burrell</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>http://dbpedia.org/resource/1699</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>http://dbpedia.org/resource/1787</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr"/>
+      <c r="E5" t="inlineStr"/>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>http://dbpedia.org/resource/Matthew_Blakiston</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>http://dbpedia.org/resource/1-1-1</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>http://dbpedia.org/resource/1-1-1</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr"/>
+      <c r="E6" t="inlineStr"/>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>http://dbpedia.org/resource/Martin_Redmayne,_Baron_Redmayne_of_Rushcliffe</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>http://dbpedia.org/resource/Martin_Redmayne,_Baron_Redmayne_of_Rushcliffe</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>http://dbpedia.org/resource/Panic_of_1910%E2%80%9311</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr"/>
+      <c r="E7" t="inlineStr"/>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>http://dbpedia.org/resource/Levinus_Bennet</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>http://dbpedia.org/resource/1-1-1</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>http://dbpedia.org/resource/1693</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr"/>
+      <c r="E8" t="inlineStr"/>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>http://dbpedia.org/resource/Leolin_Forestier-Walker</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>http://dbpedia.org/resource/1-1-1</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>http://dbpedia.org/resource/1-1-1</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr"/>
+      <c r="E9" t="inlineStr"/>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>http://dbpedia.org/resource/Lawrence_Vaughan_Palk</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>http://dbpedia.org/resource/1793</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>http://dbpedia.org/resource/1860</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr"/>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">http://dbpedia.org/resource/Exeter </t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>http://dbpedia.org/resource/Joseph_Hewitt</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>http://dbpedia.org/resource/1865</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>http://dbpedia.org/resource/1923</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr"/>
+      <c r="E11" t="inlineStr"/>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>http://dbpedia.org/resource/John_Neeld</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>http://dbpedia.org/resource/1-1-1</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>http://dbpedia.org/resource/1-1-1</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr"/>
+      <c r="E12" t="inlineStr"/>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>http://dbpedia.org/resource/John_Kinloch</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>http://dbpedia.org/resource/1-1-1</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>http://dbpedia.org/resource/1-1-1</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr"/>
+      <c r="E13" t="inlineStr"/>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>http://dbpedia.org/resource/John_Bryn_Edwards</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>http://dbpedia.org/resource/1889</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>http://dbpedia.org/resource/1922</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr"/>
+      <c r="E14" t="inlineStr"/>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>http://dbpedia.org/resource/John_Aubrey-Fletcher</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>http://dbpedia.org/resource/1912</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>http://dbpedia.org/resource/1992</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr"/>
+      <c r="E15" t="inlineStr"/>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>http://dbpedia.org/resource/John_Armytage</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>http://dbpedia.org/resource/1732</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>http://dbpedia.org/resource/1758</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr"/>
+      <c r="E16" t="inlineStr"/>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>http://dbpedia.org/resource/Jocelyn_Lucas</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>http://dbpedia.org/resource/1889</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>http://dbpedia.org/resource/5/2</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr"/>
+      <c r="E17" t="inlineStr"/>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>http://dbpedia.org/resource/James_Rushout</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>http://dbpedia.org/resource/1644</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>http://dbpedia.org/resource/1698</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr"/>
+      <c r="E18" t="inlineStr"/>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>http://dbpedia.org/resource/James_Everard_Home</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>http://dbpedia.org/resource/1798</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>http://dbpedia.org/resource/1853</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr"/>
+      <c r="E19" t="inlineStr"/>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>http://dbpedia.org/resource/James_Bellingham</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>http://dbpedia.org/resource/1623</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>http://dbpedia.org/resource/1650</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr"/>
+      <c r="E20" t="inlineStr"/>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>http://dbpedia.org/resource/Hugh_Evelyn</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>http://dbpedia.org/resource/1769</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>http://dbpedia.org/resource/1848</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr"/>
+      <c r="E21" t="inlineStr"/>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>http://dbpedia.org/resource/Herbert_Mackworth</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>http://dbpedia.org/resource/1687</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>http://dbpedia.org/resource/1765</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr"/>
+      <c r="E22" t="inlineStr"/>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>http://dbpedia.org/resource/Herbert_Cory</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>http://dbpedia.org/resource/2-2-2</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>http://dbpedia.org/resource/2-2-2</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr"/>
+      <c r="E23" t="inlineStr"/>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>http://dbpedia.org/resource/Henry_Stracey</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>http://dbpedia.org/resource/1-1-1</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>http://dbpedia.org/resource/1-1-1</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr"/>
+      <c r="E24" t="inlineStr"/>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>http://dbpedia.org/resource/Henry_Peek</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>http://dbpedia.org/resource/1825</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>http://dbpedia.org/resource/1898</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr"/>
+      <c r="E25" t="inlineStr"/>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>http://dbpedia.org/resource/Henry_Hibbert</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>http://dbpedia.org/resource/4-4-4</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>http://dbpedia.org/resource/1927</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr"/>
+      <c r="E26" t="inlineStr"/>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>http://dbpedia.org/resource/Henry_Benyon</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>http://dbpedia.org/resource/1-1-1</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>http://dbpedia.org/resource/1-1-1</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr"/>
+      <c r="E27" t="inlineStr"/>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>http://dbpedia.org/resource/Harry_Meysey-Thompson</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>http://dbpedia.org/resource/1809</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>http://dbpedia.org/resource/1874</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr"/>
+      <c r="E28" t="inlineStr"/>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>http://dbpedia.org/resource/Harry_Hope</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>http://dbpedia.org/resource/1-1-1</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>http://dbpedia.org/resource/1-1-1</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr"/>
+      <c r="E29" t="inlineStr"/>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>http://dbpedia.org/resource/Harold_Augustus_Wernher</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>http://dbpedia.org/resource/1893</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>http://dbpedia.org/resource/1973</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr"/>
+      <c r="E30" t="inlineStr"/>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>http://dbpedia.org/resource/Hardman_Lever</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>http://dbpedia.org/resource/1869</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>http://dbpedia.org/resource/1947</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr"/>
+      <c r="E31" t="inlineStr"/>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>http://dbpedia.org/resource/Hamilton_Kerr</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>http://dbpedia.org/resource/1903</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>http://dbpedia.org/resource/1974</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr"/>
+      <c r="E32" t="inlineStr"/>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>http://dbpedia.org/resource/Gregory_Foster</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>http://dbpedia.org/resource/1866</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>http://dbpedia.org/resource/1-1-1</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr"/>
+      <c r="E33" t="inlineStr"/>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>http://dbpedia.org/resource/George_Stucley</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>http://dbpedia.org/resource/1812</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>http://dbpedia.org/resource/1900</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr"/>
+      <c r="E34" t="inlineStr"/>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>http://dbpedia.org/resource/George_Sleight</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>http://dbpedia.org/resource/1853</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>http://dbpedia.org/resource/1921</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr"/>
+      <c r="E35" t="inlineStr"/>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>http://dbpedia.org/resource/George_Holcroft</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>http://dbpedia.org/resource/0-0</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>http://dbpedia.org/resource/1951</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr"/>
+      <c r="E36" t="inlineStr"/>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>http://dbpedia.org/resource/George_Clark_Williams</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>http://dbpedia.org/resource/1-1-1</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>http://dbpedia.org/resource/1-1-1</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr"/>
+      <c r="E37" t="inlineStr"/>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>http://dbpedia.org/resource/George_Bracewell_Smith</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>http://dbpedia.org/resource/12-12-12</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>http://dbpedia.org/resource/1976</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr"/>
+      <c r="E38" t="inlineStr"/>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>http://dbpedia.org/resource/George_Bisshopp</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>http://dbpedia.org/resource/1791</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>http://dbpedia.org/resource/1834</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr"/>
+      <c r="E39" t="inlineStr"/>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>http://dbpedia.org/resource/Geoffrey_Cornewall</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>http://dbpedia.org/resource/1869</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>http://dbpedia.org/resource/1951</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr"/>
+      <c r="E40" t="inlineStr"/>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>http://dbpedia.org/resource/Frederick_Milner</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>http://dbpedia.org/resource/1849</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>http://dbpedia.org/resource/1931</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr"/>
+      <c r="E41" t="inlineStr"/>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>http://dbpedia.org/resource/Frank_Sanderson</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>http://dbpedia.org/resource/1-1-1</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>http://dbpedia.org/resource/1965</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr"/>
+      <c r="E42" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Régler les problèmes de d'affichage de questions.
</commit_message>
<xml_diff>
--- a/File Name.xlsx
+++ b/File Name.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E42"/>
+  <dimension ref="A1:D42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -454,11 +454,6 @@
           <t>http://dbpedia.org/ontology/birthPlace</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>http://dbpedia.org/ontology/deathPlace</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -477,7 +472,6 @@
         </is>
       </c>
       <c r="D2" t="inlineStr"/>
-      <c r="E2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -496,7 +490,6 @@
         </is>
       </c>
       <c r="D3" t="inlineStr"/>
-      <c r="E3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -515,7 +508,6 @@
         </is>
       </c>
       <c r="D4" t="inlineStr"/>
-      <c r="E4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -534,7 +526,6 @@
         </is>
       </c>
       <c r="D5" t="inlineStr"/>
-      <c r="E5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -553,7 +544,6 @@
         </is>
       </c>
       <c r="D6" t="inlineStr"/>
-      <c r="E6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -572,7 +562,6 @@
         </is>
       </c>
       <c r="D7" t="inlineStr"/>
-      <c r="E7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -591,7 +580,6 @@
         </is>
       </c>
       <c r="D8" t="inlineStr"/>
-      <c r="E8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -610,7 +598,6 @@
         </is>
       </c>
       <c r="D9" t="inlineStr"/>
-      <c r="E9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -629,11 +616,6 @@
         </is>
       </c>
       <c r="D10" t="inlineStr"/>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t xml:space="preserve">http://dbpedia.org/resource/Exeter </t>
-        </is>
-      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -652,7 +634,6 @@
         </is>
       </c>
       <c r="D11" t="inlineStr"/>
-      <c r="E11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -671,7 +652,6 @@
         </is>
       </c>
       <c r="D12" t="inlineStr"/>
-      <c r="E12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -690,7 +670,6 @@
         </is>
       </c>
       <c r="D13" t="inlineStr"/>
-      <c r="E13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -709,7 +688,6 @@
         </is>
       </c>
       <c r="D14" t="inlineStr"/>
-      <c r="E14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -728,7 +706,6 @@
         </is>
       </c>
       <c r="D15" t="inlineStr"/>
-      <c r="E15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -747,7 +724,6 @@
         </is>
       </c>
       <c r="D16" t="inlineStr"/>
-      <c r="E16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -766,7 +742,6 @@
         </is>
       </c>
       <c r="D17" t="inlineStr"/>
-      <c r="E17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -785,7 +760,6 @@
         </is>
       </c>
       <c r="D18" t="inlineStr"/>
-      <c r="E18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -804,7 +778,6 @@
         </is>
       </c>
       <c r="D19" t="inlineStr"/>
-      <c r="E19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -823,7 +796,6 @@
         </is>
       </c>
       <c r="D20" t="inlineStr"/>
-      <c r="E20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -842,7 +814,6 @@
         </is>
       </c>
       <c r="D21" t="inlineStr"/>
-      <c r="E21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -861,7 +832,6 @@
         </is>
       </c>
       <c r="D22" t="inlineStr"/>
-      <c r="E22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -880,7 +850,6 @@
         </is>
       </c>
       <c r="D23" t="inlineStr"/>
-      <c r="E23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -899,7 +868,6 @@
         </is>
       </c>
       <c r="D24" t="inlineStr"/>
-      <c r="E24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -918,7 +886,6 @@
         </is>
       </c>
       <c r="D25" t="inlineStr"/>
-      <c r="E25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -937,7 +904,6 @@
         </is>
       </c>
       <c r="D26" t="inlineStr"/>
-      <c r="E26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -956,7 +922,6 @@
         </is>
       </c>
       <c r="D27" t="inlineStr"/>
-      <c r="E27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -975,7 +940,6 @@
         </is>
       </c>
       <c r="D28" t="inlineStr"/>
-      <c r="E28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -994,7 +958,6 @@
         </is>
       </c>
       <c r="D29" t="inlineStr"/>
-      <c r="E29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -1013,7 +976,6 @@
         </is>
       </c>
       <c r="D30" t="inlineStr"/>
-      <c r="E30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -1032,7 +994,6 @@
         </is>
       </c>
       <c r="D31" t="inlineStr"/>
-      <c r="E31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -1051,7 +1012,6 @@
         </is>
       </c>
       <c r="D32" t="inlineStr"/>
-      <c r="E32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -1070,7 +1030,6 @@
         </is>
       </c>
       <c r="D33" t="inlineStr"/>
-      <c r="E33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -1089,7 +1048,6 @@
         </is>
       </c>
       <c r="D34" t="inlineStr"/>
-      <c r="E34" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -1108,7 +1066,6 @@
         </is>
       </c>
       <c r="D35" t="inlineStr"/>
-      <c r="E35" t="inlineStr"/>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -1127,7 +1084,6 @@
         </is>
       </c>
       <c r="D36" t="inlineStr"/>
-      <c r="E36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -1146,7 +1102,6 @@
         </is>
       </c>
       <c r="D37" t="inlineStr"/>
-      <c r="E37" t="inlineStr"/>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -1165,7 +1120,6 @@
         </is>
       </c>
       <c r="D38" t="inlineStr"/>
-      <c r="E38" t="inlineStr"/>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -1184,7 +1138,6 @@
         </is>
       </c>
       <c r="D39" t="inlineStr"/>
-      <c r="E39" t="inlineStr"/>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -1203,7 +1156,6 @@
         </is>
       </c>
       <c r="D40" t="inlineStr"/>
-      <c r="E40" t="inlineStr"/>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -1222,7 +1174,6 @@
         </is>
       </c>
       <c r="D41" t="inlineStr"/>
-      <c r="E41" t="inlineStr"/>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -1241,7 +1192,6 @@
         </is>
       </c>
       <c r="D42" t="inlineStr"/>
-      <c r="E42" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Nouveaux fichiers dans le projet
</commit_message>
<xml_diff>
--- a/File Name.xlsx
+++ b/File Name.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D42"/>
+  <dimension ref="A1:C71"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -449,11 +449,6 @@
           <t>http://dbpedia.org/ontology/deathDate</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>http://dbpedia.org/ontology/birthPlace</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -471,7 +466,6 @@
           <t>http://dbpedia.org/resource/1929</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -489,7 +483,6 @@
           <t>http://dbpedia.org/resource/22_(number)</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -507,7 +500,6 @@
           <t>http://dbpedia.org/resource/1924</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -525,7 +517,6 @@
           <t>http://dbpedia.org/resource/1787</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -543,7 +534,6 @@
           <t>http://dbpedia.org/resource/1-1-1</t>
         </is>
       </c>
-      <c r="D6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -561,7 +551,6 @@
           <t>http://dbpedia.org/resource/Panic_of_1910%E2%80%9311</t>
         </is>
       </c>
-      <c r="D7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -579,7 +568,6 @@
           <t>http://dbpedia.org/resource/1693</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -597,7 +585,6 @@
           <t>http://dbpedia.org/resource/1-1-1</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -615,7 +602,6 @@
           <t>http://dbpedia.org/resource/1860</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -633,7 +619,6 @@
           <t>http://dbpedia.org/resource/1923</t>
         </is>
       </c>
-      <c r="D11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -651,7 +636,6 @@
           <t>http://dbpedia.org/resource/1-1-1</t>
         </is>
       </c>
-      <c r="D12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -669,7 +653,6 @@
           <t>http://dbpedia.org/resource/1-1-1</t>
         </is>
       </c>
-      <c r="D13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -687,7 +670,6 @@
           <t>http://dbpedia.org/resource/1922</t>
         </is>
       </c>
-      <c r="D14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -705,7 +687,6 @@
           <t>http://dbpedia.org/resource/1992</t>
         </is>
       </c>
-      <c r="D15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -723,7 +704,6 @@
           <t>http://dbpedia.org/resource/1758</t>
         </is>
       </c>
-      <c r="D16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -741,7 +721,6 @@
           <t>http://dbpedia.org/resource/5/2</t>
         </is>
       </c>
-      <c r="D17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -759,7 +738,6 @@
           <t>http://dbpedia.org/resource/1698</t>
         </is>
       </c>
-      <c r="D18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -777,7 +755,6 @@
           <t>http://dbpedia.org/resource/1853</t>
         </is>
       </c>
-      <c r="D19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -795,7 +772,6 @@
           <t>http://dbpedia.org/resource/1650</t>
         </is>
       </c>
-      <c r="D20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -813,7 +789,6 @@
           <t>http://dbpedia.org/resource/1848</t>
         </is>
       </c>
-      <c r="D21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -831,7 +806,6 @@
           <t>http://dbpedia.org/resource/1765</t>
         </is>
       </c>
-      <c r="D22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -849,7 +823,6 @@
           <t>http://dbpedia.org/resource/2-2-2</t>
         </is>
       </c>
-      <c r="D23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -867,7 +840,6 @@
           <t>http://dbpedia.org/resource/1-1-1</t>
         </is>
       </c>
-      <c r="D24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -885,7 +857,6 @@
           <t>http://dbpedia.org/resource/1898</t>
         </is>
       </c>
-      <c r="D25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -903,7 +874,6 @@
           <t>http://dbpedia.org/resource/1927</t>
         </is>
       </c>
-      <c r="D26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -921,7 +891,6 @@
           <t>http://dbpedia.org/resource/1-1-1</t>
         </is>
       </c>
-      <c r="D27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -939,7 +908,6 @@
           <t>http://dbpedia.org/resource/1874</t>
         </is>
       </c>
-      <c r="D28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -957,7 +925,6 @@
           <t>http://dbpedia.org/resource/1-1-1</t>
         </is>
       </c>
-      <c r="D29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -975,7 +942,6 @@
           <t>http://dbpedia.org/resource/1973</t>
         </is>
       </c>
-      <c r="D30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -993,7 +959,6 @@
           <t>http://dbpedia.org/resource/1947</t>
         </is>
       </c>
-      <c r="D31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -1011,7 +976,6 @@
           <t>http://dbpedia.org/resource/1974</t>
         </is>
       </c>
-      <c r="D32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -1029,7 +993,6 @@
           <t>http://dbpedia.org/resource/1-1-1</t>
         </is>
       </c>
-      <c r="D33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -1047,7 +1010,6 @@
           <t>http://dbpedia.org/resource/1900</t>
         </is>
       </c>
-      <c r="D34" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -1065,7 +1027,6 @@
           <t>http://dbpedia.org/resource/1921</t>
         </is>
       </c>
-      <c r="D35" t="inlineStr"/>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -1083,7 +1044,6 @@
           <t>http://dbpedia.org/resource/1951</t>
         </is>
       </c>
-      <c r="D36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -1101,7 +1061,6 @@
           <t>http://dbpedia.org/resource/1-1-1</t>
         </is>
       </c>
-      <c r="D37" t="inlineStr"/>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -1119,7 +1078,6 @@
           <t>http://dbpedia.org/resource/1976</t>
         </is>
       </c>
-      <c r="D38" t="inlineStr"/>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -1137,7 +1095,6 @@
           <t>http://dbpedia.org/resource/1834</t>
         </is>
       </c>
-      <c r="D39" t="inlineStr"/>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -1155,7 +1112,6 @@
           <t>http://dbpedia.org/resource/1951</t>
         </is>
       </c>
-      <c r="D40" t="inlineStr"/>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -1173,7 +1129,6 @@
           <t>http://dbpedia.org/resource/1931</t>
         </is>
       </c>
-      <c r="D41" t="inlineStr"/>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -1191,7 +1146,283 @@
           <t>http://dbpedia.org/resource/1965</t>
         </is>
       </c>
-      <c r="D42" t="inlineStr"/>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>http://dbpedia.org/resource/Francis_Freeling</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr"/>
+      <c r="C43" t="inlineStr"/>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>http://dbpedia.org/resource/Francis_Champneys</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t xml:space="preserve">1848-03-25 </t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t xml:space="preserve">1930-07-30 </t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>http://dbpedia.org/resource/Ferdinand_Dalberg-Acton</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr"/>
+      <c r="C45" t="inlineStr"/>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>http://dbpedia.org/resource/Ernest_Musgrave_Harvey</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr"/>
+      <c r="C46" t="inlineStr"/>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>http://dbpedia.org/resource/Ernest_Craig</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr"/>
+      <c r="C47" t="inlineStr"/>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>http://dbpedia.org/resource/Erik_Ohlson</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr"/>
+      <c r="C48" t="inlineStr"/>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>http://dbpedia.org/resource/Edward_des_Bouverie</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr"/>
+      <c r="C49" t="inlineStr"/>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>http://dbpedia.org/resource/Edward_Manningham-Buller</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr"/>
+      <c r="C50" t="inlineStr"/>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>http://dbpedia.org/resource/Edward_Mackay_Edgar</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr"/>
+      <c r="C51" t="inlineStr"/>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>http://dbpedia.org/resource/Edward_Irby</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr"/>
+      <c r="C52" t="inlineStr"/>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>http://dbpedia.org/resource/Edmund_Findlay</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t xml:space="preserve">1902-06-14 </t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t xml:space="preserve">1962-09-06 </t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>http://dbpedia.org/resource/Cuthbert_Ackroyd</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr"/>
+      <c r="C54" t="inlineStr"/>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>http://dbpedia.org/resource/Currimbhoy_Ebrahim</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr"/>
+      <c r="C55" t="inlineStr"/>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>http://dbpedia.org/resource/Cory_Cory-Wright</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr"/>
+      <c r="C56" t="inlineStr"/>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>http://dbpedia.org/resource/Charles_Renshaw</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr"/>
+      <c r="C57" t="inlineStr"/>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>http://dbpedia.org/resource/Charles_Jessel</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr"/>
+      <c r="C58" t="inlineStr"/>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>http://dbpedia.org/resource/Charles_Gladstone</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr"/>
+      <c r="C59" t="inlineStr"/>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>http://dbpedia.org/resource/Charles_Cornwallis_Lloyd</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr"/>
+      <c r="C60" t="inlineStr"/>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>http://dbpedia.org/resource/Brograve_Beauchamp</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr"/>
+      <c r="C61" t="inlineStr"/>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>http://dbpedia.org/resource/Bernard_Waley-Cohen</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr"/>
+      <c r="C62" t="inlineStr"/>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>http://dbpedia.org/resource/August_Cayzer</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr"/>
+      <c r="C63" t="inlineStr"/>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>http://dbpedia.org/resource/Arthur_Cory-Wright</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr"/>
+      <c r="C64" t="inlineStr"/>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>http://dbpedia.org/resource/Archibald_Birkmyre</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr"/>
+      <c r="C65" t="inlineStr"/>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>http://dbpedia.org/resource/Antony_Guy_Acland</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr"/>
+      <c r="C66" t="inlineStr"/>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>http://dbpedia.org/resource/Anthony_Aucher</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr"/>
+      <c r="C67" t="inlineStr"/>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>http://dbpedia.org/resource/Andrew_Lauder</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr"/>
+      <c r="C68" t="inlineStr"/>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>http://dbpedia.org/resource/Andrew_Armstrong</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr"/>
+      <c r="C69" t="inlineStr"/>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>http://dbpedia.org/resource/Alexander_Erskine-Hill</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr"/>
+      <c r="C70" t="inlineStr"/>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>http://dbpedia.org/resource/Abraham_Janssen</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr"/>
+      <c r="C71" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Rearrange Index Add the 3 case example files Add try catch if HttpError with MTAB Improvement Questions
</commit_message>
<xml_diff>
--- a/File Name.xlsx
+++ b/File Name.xlsx
@@ -456,7 +456,7 @@
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>http://dbpedia.org/ontology/birthDate</t>
+          <t>http://dbpedia.org/property/burialPlace</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
@@ -488,7 +488,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t xml:space="preserve">1578-10-04 </t>
+          <t>nan</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -518,8 +518,16 @@
           <t>http://dbpedia.org/resource/1642</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr"/>
-      <c r="F3" t="inlineStr"/>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -544,7 +552,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t xml:space="preserve">1784-01-12 </t>
+          <t>nan</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -574,8 +582,16 @@
           <t>http://dbpedia.org/resource/12-12-12</t>
         </is>
       </c>
-      <c r="E5" t="inlineStr"/>
-      <c r="F5" t="inlineStr"/>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -598,8 +614,16 @@
           <t>http://dbpedia.org/resource/1252</t>
         </is>
       </c>
-      <c r="E6" t="inlineStr"/>
-      <c r="F6" t="inlineStr"/>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Seville Cathedral, Seville, Spain </t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -624,7 +648,7 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t xml:space="preserve">1675-01-27 </t>
+          <t>nan</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -654,8 +678,16 @@
           <t>http://dbpedia.org/resource/1066</t>
         </is>
       </c>
-      <c r="E8" t="inlineStr"/>
-      <c r="F8" t="inlineStr"/>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t xml:space="preserve">http://dbpedia.org/resource/United_Kingdom http://dbpedia.org/resource/England http://dbpedia.org/resource/Westminster_Abbey </t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -678,8 +710,16 @@
           <t>http://dbpedia.org/resource/1864</t>
         </is>
       </c>
-      <c r="E9" t="inlineStr"/>
-      <c r="F9" t="inlineStr"/>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -704,7 +744,7 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t xml:space="preserve">1844-12-07 </t>
+          <t>nan</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
@@ -734,8 +774,16 @@
           <t>http://dbpedia.org/resource/2003</t>
         </is>
       </c>
-      <c r="E11" t="inlineStr"/>
-      <c r="F11" t="inlineStr"/>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>